<commit_message>
Update All Auddict Expression map files
</commit_message>
<xml_diff>
--- a/Auddict/xlsx/Virtuoso Violin.xlsx
+++ b/Auddict/xlsx/Virtuoso Violin.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="171">
   <si>
     <t>Name</t>
   </si>
@@ -1174,7 +1174,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1187,7 +1187,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
@@ -1244,8 +1244,12 @@
       <c r="B2" s="12">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>

</xml_diff>